<commit_message>
Documentation updated: - made a smaller one - couple of plots made
Algorithms: (test them all)
- Derivative DTW implemented
- Sakoe-Chiba band implemented
- Different step patterns implemented
</commit_message>
<xml_diff>
--- a/docs/Documentation/Ver 2/Algorithms tests comparison table in tries.xlsx
+++ b/docs/Documentation/Ver 2/Algorithms tests comparison table in tries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="14625"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Squat</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Algorithm/Action</t>
+  </si>
+  <si>
+    <t>10/11</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -499,6 +504,9 @@
       <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -518,6 +526,9 @@
       </c>
       <c r="F3" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>